<commit_message>
Changes made for Alert test
</commit_message>
<xml_diff>
--- a/Excelens_Trunk/src/com/proj/objectRepository/ObjectsFile_CorporateLens.xlsx
+++ b/Excelens_Trunk/src/com/proj/objectRepository/ObjectsFile_CorporateLens.xlsx
@@ -5,7 +5,7 @@
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Excelens_JWS\Excelens_Trunk_Jul122017\src\com\proj\objectRepository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT_EXCL_JUL\Excelens_Trunk\src\com\proj\objectRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,12 +20,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Objects_Alerts!$A$1:$G$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Objects_Documents_Toolbar!$A$1:$G$10</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="75">
   <si>
     <t>textbox</t>
   </si>
@@ -129,9 +129,6 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>User Site Menu Tool Bar</t>
-  </si>
-  <si>
     <t>xpath</t>
   </si>
   <si>
@@ -235,12 +232,30 @@
   </si>
   <si>
     <t>.//*[contains(@id,'Active_')]</t>
+  </si>
+  <si>
+    <t>Alerts</t>
+  </si>
+  <si>
+    <t>Alerts-Notification</t>
+  </si>
+  <si>
+    <t>.//*[@id='js-alertsContainer']/descendant :: div [@class='alert alert-status']/div/strong[text()='alertName']</t>
+  </si>
+  <si>
+    <t>Alerts-Notification-Tag</t>
+  </si>
+  <si>
+    <t>/../..</t>
+  </si>
+  <si>
+    <t>webelement_background_color</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -312,7 +327,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
@@ -320,6 +335,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -669,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A37"/>
+  <dimension ref="A2:A38"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:A37"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -817,47 +833,52 @@
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -874,10 +895,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -913,70 +934,98 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="A2" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7">
       <c r="B3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="B4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="B5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="B6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
         <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="B7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="B8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -984,7 +1033,7 @@
     <mergeCell ref="A2:G2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C8">
       <formula1>"id,name,xpath"</formula1>
     </dataValidation>
   </dataValidations>
@@ -998,7 +1047,7 @@
           <x14:formula1>
             <xm:f>Objects!$A$2:$A$39</xm:f>
           </x14:formula1>
-          <xm:sqref>D3:D6</xm:sqref>
+          <xm:sqref>D3:D8</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1047,153 +1096,153 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="A2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:9">
       <c r="B3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="B4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="B5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="B6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="B7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="B8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="B9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="B10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="B11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
@@ -1210,13 +1259,13 @@
       <c r="E39" s="4"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="3"/>
@@ -1224,22 +1273,22 @@
       <c r="G43" s="3"/>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Objects required for Alerts,Announcements,Blogs and My Documents are included.
</commit_message>
<xml_diff>
--- a/Excelens_Trunk/src/com/proj/objectRepository/ObjectsFile_CorporateLens.xlsx
+++ b/Excelens_Trunk/src/com/proj/objectRepository/ObjectsFile_CorporateLens.xlsx
@@ -9,23 +9,29 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20370" windowHeight="7980" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20370" windowHeight="7980" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Objects" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="Objects_Alerts" sheetId="2" r:id="rId2"/>
-    <sheet name="Objects_Documents_Toolbar" sheetId="3" r:id="rId3"/>
+    <sheet name="Objects_NewsCarousel" sheetId="4" r:id="rId3"/>
+    <sheet name="Objects_Blog" sheetId="5" r:id="rId4"/>
+    <sheet name="Objects_MyDocuments" sheetId="6" r:id="rId5"/>
+    <sheet name="Objects_Documents_Toolbar" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Objects_Alerts!$A$1:$G$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Objects_Documents_Toolbar!$A$1:$G$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Objects_Blog!$A$1:$G$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Objects_Documents_Toolbar!$A$1:$G$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Objects_MyDocuments!$A$1:$G$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Objects_NewsCarousel!$A$1:$G$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="85">
   <si>
     <t>textbox</t>
   </si>
@@ -250,6 +256,36 @@
   </si>
   <si>
     <t>webelement_background_color</t>
+  </si>
+  <si>
+    <t>Home Page -NewsCarousel Article</t>
+  </si>
+  <si>
+    <t>NewsCarousel</t>
+  </si>
+  <si>
+    <t>.//*[@class='newsCarouselItems__item']/descendant ::h1 [text()='tile']</t>
+  </si>
+  <si>
+    <t>Home Page -Blog Article</t>
+  </si>
+  <si>
+    <t>.//*[@class='atWidget__header atWidget__header--icon' and text()='Blogs']/../../div/descendant ::div[@class='row']/div[2]/h4[text()='tile']</t>
+  </si>
+  <si>
+    <t>Blog</t>
+  </si>
+  <si>
+    <t>.//*[@class='atWidget__header']/../descendant :: li/a[@title='documentName']</t>
+  </si>
+  <si>
+    <t>Home Page -My Document</t>
+  </si>
+  <si>
+    <t>webelement_notdisplayed</t>
+  </si>
+  <si>
+    <t>Home Page -My Document-Visitor/Other Contributor</t>
   </si>
 </sst>
 </file>
@@ -685,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A38"/>
+  <dimension ref="A2:A39"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -879,6 +915,11 @@
     <row r="38" spans="1:1">
       <c r="A38" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -897,7 +938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -1045,7 +1086,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Objects!$A$2:$A$39</xm:f>
+            <xm:f>Objects!$A$2:$A$38</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D8</xm:sqref>
         </x14:dataValidation>
@@ -1056,6 +1097,296 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="44.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="41.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:G2"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
+      <formula1>"id,name,xpath"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Objects!$A$2:$A$38</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="44.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="41.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:G2"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
+      <formula1>"id,name,xpath"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Objects!$A$2:$A$38</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="44.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="41.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:G2"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C4">
+      <formula1>"id,name,xpath"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Objects!$A$2:$A$100</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3:D4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I47"/>
   <sheetViews>
@@ -1308,12 +1639,42 @@
   <headerFooter alignWithMargins="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Objects!$A$2:$A$39</xm:f>
+            <xm:f>Objects!$A$2:$A$38</xm:f>
           </x14:formula1>
-          <xm:sqref>D40 D42:D43 D16:D30 D45 D48 D3:D14</xm:sqref>
+          <xm:sqref>D40</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Objects!$A$2:$A$38</xm:f>
+          </x14:formula1>
+          <xm:sqref>D42:D43</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Objects!$A$2:$A$38</xm:f>
+          </x14:formula1>
+          <xm:sqref>D16:D30</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Objects!$A$2:$A$38</xm:f>
+          </x14:formula1>
+          <xm:sqref>D45</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Objects!$A$2:$A$38</xm:f>
+          </x14:formula1>
+          <xm:sqref>D48</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Objects!$A$2:$A$38</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3:D14</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Updated/Included required objects for favourites tests
</commit_message>
<xml_diff>
--- a/Excelens_Trunk/src/com/proj/objectRepository/ObjectsFile_CorporateLens.xlsx
+++ b/Excelens_Trunk/src/com/proj/objectRepository/ObjectsFile_CorporateLens.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20370" windowHeight="7980" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20370" windowHeight="7980" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Objects" sheetId="1" state="hidden" r:id="rId1"/>
@@ -17,12 +17,14 @@
     <sheet name="Objects_NewsCarousel" sheetId="4" r:id="rId3"/>
     <sheet name="Objects_Blog" sheetId="5" r:id="rId4"/>
     <sheet name="Objects_MyDocuments" sheetId="6" r:id="rId5"/>
-    <sheet name="Objects_Documents_Toolbar" sheetId="3" r:id="rId6"/>
+    <sheet name="Objects_Favourites" sheetId="7" r:id="rId6"/>
+    <sheet name="Objects_Documents_Toolbar" sheetId="3" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Objects_Alerts!$A$1:$G$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Objects_Blog!$A$1:$G$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Objects_Documents_Toolbar!$A$1:$G$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Objects_Documents_Toolbar!$A$1:$G$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Objects_Favourites!$A$1:$G$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Objects_MyDocuments!$A$1:$G$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Objects_NewsCarousel!$A$1:$G$2</definedName>
   </definedNames>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="109">
   <si>
     <t>textbox</t>
   </si>
@@ -286,6 +288,78 @@
   </si>
   <si>
     <t>Home Page -My Document-Visitor/Other Contributor</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>.//*[contains(@id,'UrlFieldUrl')]</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>.//*[contains(@id,'UrlFieldDescription')]</t>
+  </si>
+  <si>
+    <t>My Favourites -Heading</t>
+  </si>
+  <si>
+    <t>Manage My Favourites -Available Items-Favourite</t>
+  </si>
+  <si>
+    <t>.//*[@data-title='tile']</t>
+  </si>
+  <si>
+    <t>Favourite-Save</t>
+  </si>
+  <si>
+    <t>.//*[@id='submit']</t>
+  </si>
+  <si>
+    <t>Create Favourite</t>
+  </si>
+  <si>
+    <t>.//*[@id='js-showForm']</t>
+  </si>
+  <si>
+    <t>Admin Favourites</t>
+  </si>
+  <si>
+    <t>My Favourites</t>
+  </si>
+  <si>
+    <t>My Favourite-Title</t>
+  </si>
+  <si>
+    <t>My Favourite-URL</t>
+  </si>
+  <si>
+    <t>My Favourite-Create</t>
+  </si>
+  <si>
+    <t>.//*[@value='Create']</t>
+  </si>
+  <si>
+    <t>.//*[@id='field_title']</t>
+  </si>
+  <si>
+    <t>.//*[@id='field_url']</t>
+  </si>
+  <si>
+    <t>.//*[contains(@class,'atWidget__header') and text()='My favourites']/../../../descendant ::li/a/h4[text()='title']</t>
+  </si>
+  <si>
+    <t>Home Page-My Favourites for Owner</t>
+  </si>
+  <si>
+    <t>Home Page-My Favourites for Non Owner</t>
+  </si>
+  <si>
+    <t>.//*[contains(@class,'atWidget__header') and text()='My favourites']/span</t>
   </si>
 </sst>
 </file>
@@ -1284,8 +1358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1355,8 +1429,9 @@
       <c r="D4" t="s">
         <v>83</v>
       </c>
-      <c r="E4" t="s">
-        <v>81</v>
+      <c r="E4" t="str">
+        <f>E3</f>
+        <v>.//*[@class='atWidget__header']/../descendant :: li/a[@title='documentName']</v>
       </c>
     </row>
   </sheetData>
@@ -1387,6 +1462,264 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="44.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="41.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="B4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="B5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="B6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="B7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="B10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="B11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="B12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="B14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="B15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A9:G9"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C5 C12:C16">
+      <formula1>"id,name,xpath"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Objects!$A$2:$A$100</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3:D7 D10:D16</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I47"/>
   <sheetViews>

</xml_diff>

<commit_message>
Changed the objects required for Calendar event and before tests.
</commit_message>
<xml_diff>
--- a/Excelens_Trunk/src/com/proj/objectRepository/ObjectsFile_CorporateLens.xlsx
+++ b/Excelens_Trunk/src/com/proj/objectRepository/ObjectsFile_CorporateLens.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20370" windowHeight="7980" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20370" windowHeight="7980" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Objects" sheetId="1" state="hidden" r:id="rId1"/>
@@ -19,13 +19,18 @@
     <sheet name="Objects_MyDocuments" sheetId="6" r:id="rId5"/>
     <sheet name="Objects_Favourites" sheetId="7" r:id="rId6"/>
     <sheet name="Objects_Announcements" sheetId="8" r:id="rId7"/>
-    <sheet name="Objects_Documents_Toolbar" sheetId="3" r:id="rId8"/>
+    <sheet name="Objects_Calendar" sheetId="9" r:id="rId8"/>
+    <sheet name="Objects_Documents_Toolbar" sheetId="3" r:id="rId9"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId10"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Objects_Alerts!$A$1:$G$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Objects_Announcements!$A$1:$G$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Objects_Blog!$A$1:$G$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Objects_Documents_Toolbar!$A$1:$G$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Objects_Calendar!$A$1:$G$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Objects_Documents_Toolbar!$A$1:$G$10</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Objects_Favourites!$A$1:$G$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Objects_MyDocuments!$A$1:$G$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Objects_NewsCarousel!$A$1:$G$2</definedName>
@@ -35,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="159">
   <si>
     <t>textbox</t>
   </si>
@@ -374,6 +379,144 @@
   </si>
   <si>
     <t>.//*[contains(@class,'atWidget__header') and text()='Announcements']/../../../descendant ::li/a/h4[text()='title']/../span[@class='icon__status fa fa-exclamation-triangle']</t>
+  </si>
+  <si>
+    <t>Calendar</t>
+  </si>
+  <si>
+    <t>.//*[contains(@class,'atWidget__header') and text()='Calendar']</t>
+  </si>
+  <si>
+    <t>.//*[@summary='Monthly graphical Calendar View']/tbody/tr[@class='ms-acal-summary-dayrow']/td[@date='eventDate']</t>
+  </si>
+  <si>
+    <t>webelement_click</t>
+  </si>
+  <si>
+    <t>Calendar -Date for Event</t>
+  </si>
+  <si>
+    <t>Calendar -Heading</t>
+  </si>
+  <si>
+    <t>Calendar-Add</t>
+  </si>
+  <si>
+    <t>.//*[@title='Add']</t>
+  </si>
+  <si>
+    <t>Calender Event-Title</t>
+  </si>
+  <si>
+    <t>Calendar Event-Location</t>
+  </si>
+  <si>
+    <t>.//*[contains(@title,'Location')]</t>
+  </si>
+  <si>
+    <t>Calendar Event-Start Time</t>
+  </si>
+  <si>
+    <t>.//*[contains(@title,'Start Time')]</t>
+  </si>
+  <si>
+    <t>Calendar Event-End Time</t>
+  </si>
+  <si>
+    <t>.//*[contains(@title,'End Time')]</t>
+  </si>
+  <si>
+    <t>Calendar Event-Start Hours</t>
+  </si>
+  <si>
+    <t>(.//*[contains(@id,'DateTimeField_DateTimeFieldDateHours')])[1]</t>
+  </si>
+  <si>
+    <t>Calendar Event-End Hours</t>
+  </si>
+  <si>
+    <t>(.//*[contains(@id,'DateTimeField_DateTimeFieldDateHours')])[2]</t>
+  </si>
+  <si>
+    <t>Calendar Event-Description</t>
+  </si>
+  <si>
+    <t>.//*[contains(@id,'TextField_inplacerte') and @role='textbox']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calendar Event-Category </t>
+  </si>
+  <si>
+    <t>Calendar Event-Category option</t>
+  </si>
+  <si>
+    <t>Calendar Event-Specify Your Own Value</t>
+  </si>
+  <si>
+    <t>.//*[@value='FillInButton' and @type='radio']</t>
+  </si>
+  <si>
+    <t>.//*[@value='DropDownButton' and @type='radio']</t>
+  </si>
+  <si>
+    <t>.//*[contains(@id,'DropDownChoice')]</t>
+  </si>
+  <si>
+    <t>.//*[contains(@title,'Category : Specify your own value:')]</t>
+  </si>
+  <si>
+    <t>Calendar Event-Specify Your Own Value Details</t>
+  </si>
+  <si>
+    <t>Calendar Event-All Day Event</t>
+  </si>
+  <si>
+    <t>.//*[contains(@id,'AllDayEventField') and @type='checkbox']</t>
+  </si>
+  <si>
+    <t>.//*[contains(@id,'RecurrenceField') and @type='checkbox']</t>
+  </si>
+  <si>
+    <t>Calendar Event-Recurrence</t>
+  </si>
+  <si>
+    <t>.//*[contains(@id,'Lookup')]</t>
+  </si>
+  <si>
+    <t>Calendar Event-Event Page</t>
+  </si>
+  <si>
+    <t>Calendar Event- more item</t>
+  </si>
+  <si>
+    <t>.//*[@class='ms-cal-nav' and contains (text(),'more item')]</t>
+  </si>
+  <si>
+    <t>Calendar Event in Calendar</t>
+  </si>
+  <si>
+    <t>.//*[@class='ms-acal-item' and contains(@title,'starthours - endhours tile')]</t>
+  </si>
+  <si>
+    <t>Calendar WebPart</t>
+  </si>
+  <si>
+    <t>.//*[contains(@class,'atWidget__header') and text()='Calendar']/../../../descendant ::li/a/h4[text()='title']</t>
+  </si>
+  <si>
+    <t>Home Page-Calendar Day Icon</t>
+  </si>
+  <si>
+    <t>Home Page-Calendar Month Icon</t>
+  </si>
+  <si>
+    <t>Home Page-Calendar Event</t>
+  </si>
+  <si>
+    <t>.//*[contains(@class,'atWidget__header') and text()='Calendar']/../../../descendant ::li/a/h4[text()='title']/../descendant :: span[text()='startday']</t>
+  </si>
+  <si>
+    <t>.//*[contains(@class,'atWidget__header') and text()='Calendar']/../../../descendant ::li/a/h4[text()='title']/../descendant :: span[text()='startmonth']</t>
   </si>
 </sst>
 </file>
@@ -478,6 +621,31 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Objects"/>
+      <sheetName val="Objects_SiteContents"/>
+      <sheetName val="Objects_Page"/>
+      <sheetName val="Objects_App"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2">
+        <row r="8">
+          <cell r="E8" t="str">
+            <v>.//*[contains(@title,'Title')]</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -809,10 +977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A39"/>
+  <dimension ref="A2:A40"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:XFD39"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1008,6 +1176,11 @@
     <row r="39" spans="1:1">
       <c r="A39" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1480,7 +1653,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1528,21 +1701,21 @@
     </row>
     <row r="3" spans="1:7">
       <c r="B3" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="B4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C4" t="s">
         <v>34</v>
@@ -1551,12 +1724,12 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>87</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="B5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
         <v>34</v>
@@ -1565,21 +1738,21 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="B6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
         <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1711,7 +1884,7 @@
     <mergeCell ref="A9:G9"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C5 C12:C16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12:C16 C4 C5:C6">
       <formula1>"id,name,xpath"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1725,7 +1898,7 @@
           <x14:formula1>
             <xm:f>Objects!$A$2:$A$100</xm:f>
           </x14:formula1>
-          <xm:sqref>D3:D7 D10:D16</xm:sqref>
+          <xm:sqref>D10:D16 D3:D6 D7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1737,8 +1910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1817,7 +1990,7 @@
     <mergeCell ref="A2:G2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C4">
       <formula1>"id,name,xpath"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1840,6 +2013,405 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="44.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="41.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="B4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="B5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" t="str">
+        <f>[1]Objects_Page!$E$8</f>
+        <v>.//*[contains(@title,'Title')]</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="B6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="B7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="B8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="B9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="B10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="B11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="B12" t="s">
+        <v>134</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" t="s">
+        <v>135</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="B14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="B15" t="s">
+        <v>141</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" t="s">
+        <v>142</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="B17" t="s">
+        <v>145</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="B18" t="s">
+        <v>147</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="B19" t="s">
+        <v>148</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="B20" t="s">
+        <v>150</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="B22" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="B23" t="s">
+        <v>156</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="B24" t="s">
+        <v>154</v>
+      </c>
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="B25" t="s">
+        <v>155</v>
+      </c>
+      <c r="C25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A21:G21"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C19 C22:C24">
+      <formula1>"id,name,xpath"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Objects!$A$2:$A$100</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3:D20 D22:D23</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I47"/>
   <sheetViews>

</xml_diff>